<commit_message>
Created a single unified input data frame for eating behavior and weight loss analyses. The data frame contains the baseline and absolute final measurements, several adaptable time window measurements, time-to-event data on achieving defined weight loss targets, basic clinical data together with eating behavior and weight gain cause data as well as the corresponding genomics sample IDs.
</commit_message>
<xml_diff>
--- a/paper1_emotional/sa_input_structure_ideation.xlsx
+++ b/paper1_emotional/sa_input_structure_ideation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="140">
   <si>
     <r>
       <t>patient_id</t>
@@ -531,9 +531,6 @@
     <t>wl_60d_%</t>
   </si>
   <si>
-    <t>80d_weight</t>
-  </si>
-  <si>
     <t>wl_80d_kg</t>
   </si>
   <si>
@@ -640,6 +637,39 @@
   </si>
   <si>
     <t>as of fil weight</t>
+  </si>
+  <si>
+    <t>patient_ID</t>
+  </si>
+  <si>
+    <t>medical_record_ID</t>
+  </si>
+  <si>
+    <t>total_followup_days</t>
+  </si>
+  <si>
+    <t>baseline_weight_kg</t>
+  </si>
+  <si>
+    <t>last_aval_weight_kg</t>
+  </si>
+  <si>
+    <t>40d_weight_kg</t>
+  </si>
+  <si>
+    <t>60d_weight_kg</t>
+  </si>
+  <si>
+    <t>80d_weight_kg</t>
+  </si>
+  <si>
+    <t>5%_wl_achieved</t>
+  </si>
+  <si>
+    <t>10%_wl_achieved</t>
+  </si>
+  <si>
+    <t>15%_wl_achieved</t>
   </si>
 </sst>
 </file>
@@ -1010,8 +1040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AW48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H27" workbookViewId="0">
-      <selection activeCell="P43" sqref="P43"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1025,7 +1055,7 @@
   <sheetData>
     <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="29">
@@ -1048,7 +1078,7 @@
         <v>4</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>5</v>
@@ -1081,10 +1111,10 @@
         <v>14</v>
       </c>
       <c r="R3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>15</v>
@@ -1182,10 +1212,10 @@
         <v>25</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>27</v>
@@ -1256,10 +1286,10 @@
     </row>
     <row r="15" spans="1:29" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>129</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>130</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>37</v>
@@ -1292,10 +1322,10 @@
         <v>43</v>
       </c>
       <c r="M15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="N15" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>46</v>
@@ -1331,10 +1361,10 @@
         <v>14</v>
       </c>
       <c r="Z15" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA15" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="AA15" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="AB15" s="1" t="s">
         <v>15</v>
@@ -1470,10 +1500,10 @@
         <v>61</v>
       </c>
       <c r="M17" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="N17" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="O17" s="2" t="s">
         <v>69</v>
@@ -1508,7 +1538,7 @@
     </row>
     <row r="22" spans="1:49">
       <c r="A22" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:49">
@@ -1517,10 +1547,10 @@
     </row>
     <row r="24" spans="1:49" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>35</v>
+        <v>129</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>36</v>
+        <v>130</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>37</v>
@@ -1529,13 +1559,13 @@
         <v>38</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>49</v>
+        <v>131</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>39</v>
+        <v>132</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>40</v>
+        <v>133</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>56</v>
@@ -1544,7 +1574,7 @@
         <v>57</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>77</v>
+        <v>134</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>78</v>
@@ -1553,16 +1583,16 @@
         <v>79</v>
       </c>
       <c r="M24" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N24" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>86</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="Q24" s="1" t="s">
         <v>91</v>
@@ -1571,34 +1601,34 @@
         <v>92</v>
       </c>
       <c r="S24" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="T24" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="T24" s="1" t="s">
+      <c r="U24" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="V24" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="W24" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="X24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y24" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="U24" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="V24" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="W24" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="X24" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y24" s="1" t="s">
+      <c r="Z24" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="Z24" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="AA24" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AB24" s="1" t="s">
-        <v>44</v>
+        <v>137</v>
       </c>
       <c r="AC24" s="1" t="s">
         <v>45</v>
@@ -1610,7 +1640,7 @@
         <v>85</v>
       </c>
       <c r="AF24" s="1" t="s">
-        <v>81</v>
+        <v>138</v>
       </c>
       <c r="AG24" s="1" t="s">
         <v>82</v>
@@ -1619,19 +1649,19 @@
         <v>83</v>
       </c>
       <c r="AI24" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AJ24" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AK24" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AK24" s="1" t="s">
+      <c r="AL24" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AL24" s="1" t="s">
+      <c r="AM24" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="AM24" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="AN24" s="1" t="s">
         <v>9</v>
@@ -1652,10 +1682,10 @@
         <v>14</v>
       </c>
       <c r="AT24" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AU24" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="AU24" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="AV24" s="1" t="s">
         <v>15</v>
@@ -1666,10 +1696,10 @@
     </row>
     <row r="25" spans="1:49">
       <c r="A25" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C25" s="5">
         <v>45658</v>
@@ -1815,10 +1845,10 @@
     </row>
     <row r="26" spans="1:49">
       <c r="A26" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="C26" s="5">
         <v>45658</v>
@@ -1869,13 +1899,13 @@
         <v>1</v>
       </c>
       <c r="AN26" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AO26" s="2">
         <v>60</v>
       </c>
       <c r="AP26" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AQ26" s="2">
         <v>42</v>
@@ -1901,12 +1931,12 @@
     </row>
     <row r="28" spans="1:49">
       <c r="A28" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:49">
       <c r="A30" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:49" s="1" customFormat="1" ht="13.5" customHeight="1">
@@ -1947,10 +1977,10 @@
         <v>79</v>
       </c>
       <c r="M31" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N31" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="N31" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="O31" s="1" t="s">
         <v>86</v>
@@ -1986,10 +2016,10 @@
         <v>14</v>
       </c>
       <c r="Z31" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA31" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="AA31" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="AB31" s="1" t="s">
         <v>15</v>
@@ -2000,10 +2030,10 @@
     </row>
     <row r="32" spans="1:49">
       <c r="A32" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C32" s="5">
         <v>45658</v>
@@ -2089,10 +2119,10 @@
     </row>
     <row r="33" spans="1:29">
       <c r="A33" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="C33" s="5">
         <v>45658</v>
@@ -2131,13 +2161,13 @@
         <v>20</v>
       </c>
       <c r="T33" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="U33" s="2">
         <v>60</v>
       </c>
       <c r="V33" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="W33" s="2">
         <v>42</v>
@@ -2168,7 +2198,7 @@
     </row>
     <row r="35" spans="1:29">
       <c r="A35" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:29" s="1" customFormat="1" ht="13.5" customHeight="1">
@@ -2209,10 +2239,10 @@
         <v>79</v>
       </c>
       <c r="M36" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N36" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="N36" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="O36" s="1" t="s">
         <v>86</v>
@@ -2227,7 +2257,7 @@
         <v>83</v>
       </c>
       <c r="S36" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T36" s="1" t="s">
         <v>9</v>
@@ -2248,10 +2278,10 @@
         <v>14</v>
       </c>
       <c r="Z36" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA36" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="AA36" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="AB36" s="1" t="s">
         <v>15</v>
@@ -2262,10 +2292,10 @@
     </row>
     <row r="37" spans="1:29">
       <c r="A37" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C37" s="5">
         <v>45658</v>
@@ -2351,10 +2381,10 @@
     </row>
     <row r="38" spans="1:29">
       <c r="A38" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="C38" s="5">
         <v>45658</v>
@@ -2384,13 +2414,13 @@
         <v>0</v>
       </c>
       <c r="T38" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="U38" s="2">
         <v>60</v>
       </c>
       <c r="V38" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="W38" s="2">
         <v>42</v>
@@ -2416,7 +2446,7 @@
     </row>
     <row r="40" spans="1:29">
       <c r="A40" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:29" s="1" customFormat="1" ht="13.5" customHeight="1">
@@ -2457,25 +2487,25 @@
         <v>79</v>
       </c>
       <c r="M41" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N41" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="N41" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="O41" s="1" t="s">
         <v>86</v>
       </c>
       <c r="P41" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q41" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="Q41" s="1" t="s">
+      <c r="R41" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="R41" s="1" t="s">
+      <c r="S41" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="S41" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="T41" s="1" t="s">
         <v>9</v>
@@ -2496,10 +2526,10 @@
         <v>14</v>
       </c>
       <c r="Z41" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA41" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="AA41" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="AB41" s="1" t="s">
         <v>15</v>
@@ -2510,10 +2540,10 @@
     </row>
     <row r="42" spans="1:29">
       <c r="A42" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C42" s="5">
         <v>45658</v>
@@ -2599,10 +2629,10 @@
     </row>
     <row r="43" spans="1:29">
       <c r="A43" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="C43" s="5">
         <v>45658</v>
@@ -2632,13 +2662,13 @@
         <v>1</v>
       </c>
       <c r="T43" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="U43" s="2">
         <v>60</v>
       </c>
       <c r="V43" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="W43" s="2">
         <v>42</v>
@@ -2668,7 +2698,7 @@
     </row>
     <row r="45" spans="1:29">
       <c r="A45" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="46" spans="1:29" s="1" customFormat="1" ht="13.5" customHeight="1">
@@ -2709,13 +2739,13 @@
         <v>92</v>
       </c>
       <c r="M46" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="N46" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="N46" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="O46" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P46" s="1" t="s">
         <v>44</v>
@@ -2748,10 +2778,10 @@
         <v>14</v>
       </c>
       <c r="Z46" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA46" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="AA46" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="AB46" s="1" t="s">
         <v>15</v>
@@ -2762,10 +2792,10 @@
     </row>
     <row r="47" spans="1:29">
       <c r="A47" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C47" s="5">
         <v>45658</v>
@@ -2851,10 +2881,10 @@
     </row>
     <row r="48" spans="1:29">
       <c r="A48" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="C48" s="5">
         <v>45658</v>
@@ -2893,13 +2923,13 @@
         <v>20</v>
       </c>
       <c r="T48" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="U48" s="2">
         <v>60</v>
       </c>
       <c r="V48" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="W48" s="2">
         <v>42</v>

</xml_diff>